<commit_message>
SearchParameter pour récupérer les offres rattachées à un professionnel (#455)
* update spec 3

* Update input/pagecontent/specifications_techniques_3.md

Co-authored-by: sdemeyANS <117643165+sdemeyANS@users.noreply.github.com>

---------

Co-authored-by: sdemeyANS <117643165+sdemeyANS@users.noreply.github.com> d09263543fdc0a48dbd2f181a8f971e4ddd2a9a8
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-ror-healthcareservice-sensitive-unit.xlsx
+++ b/main/ig/StructureDefinition-ror-healthcareservice-sensitive-unit.xlsx
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-20T13:10:13+00:00</t>
+    <t>2026-01-21T15:54:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -78,7 +78,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension créée dans le cadre du ROR pour signaler que toutes les informations de description d'une offre sont confidentielles car elles présentent un risque d'utilisation à des fins malveillantes.</t>
+    <t>Extension créée dans le cadre du ROR pour signaler que toutes les informations de description d'une offre sont confidentielles car elles présentent un risque d'utilisation à des fins malveillantes, ou que le porteur d'offre ne souhaite pas diffuser.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>